<commit_message>
Updated the first figure to show proper coord system and implicit assumpts
</commit_message>
<xml_diff>
--- a/CaseStudies/projectileLesson/InformationCapturedInArtifacts.xlsx
+++ b/CaseStudies/projectileLesson/InformationCapturedInArtifacts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/smiths/Repos/caseStudies/CaseStudies/projectileLesson/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F169C8D-0A5C-8B46-8689-CB43A65202A5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A651BEA-DDFC-3A4E-B834-70F853995AA1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1820" yWindow="3240" windowWidth="28040" windowHeight="17440" xr2:uid="{07A599C7-DCE0-8F49-95F0-93069E100C22}"/>
+    <workbookView xWindow="25320" yWindow="8060" windowWidth="28040" windowHeight="17440" xr2:uid="{07A599C7-DCE0-8F49-95F0-93069E100C22}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="69">
   <si>
     <t>Information Embedded in the Projectile Example</t>
   </si>
@@ -139,13 +139,115 @@
   </si>
   <si>
     <t xml:space="preserve">string X string -&gt; string </t>
+  </si>
+  <si>
+    <t>…</t>
+  </si>
+  <si>
+    <t>Comparison of Drasil SRS and Projectile Lesson Jupyter lab</t>
+  </si>
+  <si>
+    <t>Chunk in Drasil SRS</t>
+  </si>
+  <si>
+    <t>Corresponding chunk in Projectile</t>
+  </si>
+  <si>
+    <t>GD:rectVel</t>
+  </si>
+  <si>
+    <t>Equation 1 (equation numbers don't currently appear in Jupyter labs)</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>Same equation, same symbols</t>
+  </si>
+  <si>
+    <t>GD:rectPos</t>
+  </si>
+  <si>
+    <t>Equation 2 (equation numbers don't currently appear in Jupyter labs)</t>
+  </si>
+  <si>
+    <t>Equation 3 (equation numbers don't currently appear in Jupyter labs)</t>
+  </si>
+  <si>
+    <t>doesn't appear in SRS</t>
+  </si>
+  <si>
+    <t>Eq 3 is derived from Eq 1 and 2, since it isn't an independent equation it wasn't given in the original SRS - the projectile lesson is actually for a family of related physics problems, not for one specific problem</t>
+  </si>
+  <si>
+    <t>Assumption: 2D Motion</t>
+  </si>
+  <si>
+    <t>explicitly stated</t>
+  </si>
+  <si>
+    <t>Assumption: cartSyst</t>
+  </si>
+  <si>
+    <t>Assumption: launchOrigin</t>
+  </si>
+  <si>
+    <t>Assumption: yAxisGravity</t>
+  </si>
+  <si>
+    <t>Assumption: targetXAxis</t>
+  </si>
+  <si>
+    <t>Assumption: posXDirection</t>
+  </si>
+  <si>
+    <t>Assumption: constAccel</t>
+  </si>
+  <si>
+    <t>Assumption: accelXZero</t>
+  </si>
+  <si>
+    <t>Assumption: accelYGravity</t>
+  </si>
+  <si>
+    <t>Assumption: neglectDrag</t>
+  </si>
+  <si>
+    <t>Assumption: pointMass</t>
+  </si>
+  <si>
+    <t>Assumption: freeFlight</t>
+  </si>
+  <si>
+    <t>Assumption: neglectCurv</t>
+  </si>
+  <si>
+    <t>Assumption: timeStartZero</t>
+  </si>
+  <si>
+    <t>Assumption: gravAccelValue</t>
+  </si>
+  <si>
+    <t>implicitly assumed</t>
+  </si>
+  <si>
+    <t>Assumption: gravNotVaryWithAltitude (unintentionally omitted)</t>
+  </si>
+  <si>
+    <t>Included in lesson, but unintentionally omitted from Drasil SRS</t>
+  </si>
+  <si>
+    <t>it isn't stated as an assumption, but the 2D Cartesian coord system figure makes it clear that 2D is being assummed</t>
+  </si>
+  <si>
+    <t>not assumed by projectile lesson, done in SRS to simplify equations; projectile lesson is more general</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -157,6 +259,13 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -182,12 +291,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -504,16 +618,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{307A6078-F65A-6142-BC1E-302ECAD836B8}">
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="54.1640625" customWidth="1"/>
-    <col min="2" max="3" width="44.5" customWidth="1"/>
+    <col min="2" max="2" width="53.5" customWidth="1"/>
+    <col min="3" max="3" width="51.1640625" customWidth="1"/>
     <col min="4" max="5" width="39.5" customWidth="1"/>
     <col min="6" max="6" width="45.1640625" customWidth="1"/>
     <col min="7" max="8" width="39.5" customWidth="1"/>
@@ -532,16 +647,16 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
@@ -588,7 +703,7 @@
       <c r="E7" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="F7" s="2" t="s">
         <v>23</v>
       </c>
       <c r="G7" t="s">
@@ -643,7 +758,7 @@
       <c r="C9" t="s">
         <v>34</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="2" t="s">
         <v>30</v>
       </c>
       <c r="E9" t="s">
@@ -663,6 +778,203 @@
       </c>
       <c r="J9" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A18" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C18" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="68" x14ac:dyDescent="0.2">
+      <c r="A19" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A20" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B20" t="s">
+        <v>64</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B21" t="s">
+        <v>64</v>
+      </c>
+      <c r="C21" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B22" t="s">
+        <v>64</v>
+      </c>
+      <c r="C22" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A23" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B23" t="s">
+        <v>64</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B24" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>55</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>56</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>57</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>58</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>59</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>60</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>61</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>62</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>63</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>65</v>
+      </c>
+      <c r="B35" t="s">
+        <v>49</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>